<commit_message>
hoop verschoven in het epi model
</commit_message>
<xml_diff>
--- a/results/selected results.xlsx
+++ b/results/selected results.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms\OneDrive\Documenten\SeminarFinance\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -25,15 +30,9 @@
     <t>Comm. real estate p (y-o-y %ch)</t>
   </si>
   <si>
-    <t>Debt/gdp</t>
-  </si>
-  <si>
     <t>Federal funds effective rate</t>
   </si>
   <si>
-    <t>Financial assets/gdp: nonfin. corp.</t>
-  </si>
-  <si>
     <t>GDP GROWTH</t>
   </si>
   <si>
@@ -43,7 +42,13 @@
     <t>KCFSI</t>
   </si>
   <si>
-    <t>VIX</t>
+    <t>log-Debt/gdp</t>
+  </si>
+  <si>
+    <t>log-Financial assets/gdp: nonfin. corp.</t>
+  </si>
+  <si>
+    <t>log-Total debt/equity: nonfin. corp.</t>
   </si>
   <si>
     <t>DFS_leverage</t>
@@ -73,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,24 +131,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" textRotation="30"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="30"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,9 +203,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +237,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,9 +272,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -424,371 +448,880 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="C2:L13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C2">
-        <v>-0.0624482023811982</v>
+        <f>ROUND(C15,3)</f>
+        <v>0.23699999999999999</v>
       </c>
       <c r="D2">
-        <v>-0.0369602303914314</v>
+        <f t="shared" ref="D2:H2" si="0">ROUND(D15,3)</f>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E2">
-        <v>0.00491558324737301</v>
+        <f t="shared" si="0"/>
+        <v>0.64600000000000002</v>
       </c>
       <c r="F2">
-        <v>0.0204583571531675</v>
+        <f t="shared" si="0"/>
+        <v>0.222</v>
       </c>
       <c r="G2">
-        <v>0.00628570484971425</v>
+        <f t="shared" si="0"/>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="H2">
-        <v>0.0138992535723278</v>
+        <f t="shared" si="0"/>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="I2">
-        <v>7.6375416230712e-05</v>
+        <f>ROUND(I15,3)</f>
+        <v>-1.5780000000000001</v>
       </c>
       <c r="J2">
-        <v>0.00346192094057223</v>
+        <f>ROUND(J15,3)</f>
+        <v>-0.04</v>
       </c>
       <c r="K2">
-        <v>-0.0610365695729597</v>
+        <f>ROUND(K15,3)</f>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0.00850825369084236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1"/>
+        <f>ROUND(L15,3)</f>
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3">
-        <v>-0.0383660446920876</v>
+        <f t="shared" ref="C3:H13" si="1">ROUND(C16,3)</f>
+        <v>0.38200000000000001</v>
       </c>
       <c r="D3">
-        <v>0.0126602401425831</v>
-      </c>
-      <c r="K3">
-        <v>-0.324575115673774</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>-0.123</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>-8.3000000000000004E-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>-0.153</v>
+      </c>
+      <c r="I3">
+        <f>ROUND(I16,3)</f>
+        <v>0.114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C4">
-        <v>-4.62812204165583</v>
+        <f t="shared" si="1"/>
+        <v>-9.4079999999999995</v>
       </c>
       <c r="D4">
-        <v>-8.28144344038629</v>
+        <f t="shared" si="1"/>
+        <v>-18.094999999999999</v>
       </c>
       <c r="E4">
-        <v>0.164330276980303</v>
+        <f t="shared" si="1"/>
+        <v>0.113</v>
       </c>
       <c r="F4">
-        <v>1.39653764369137</v>
+        <f t="shared" si="1"/>
+        <v>-3.0169999999999999</v>
       </c>
       <c r="G4">
-        <v>0.181787365932496</v>
+        <f t="shared" si="1"/>
+        <v>-3.7989999999999999</v>
       </c>
       <c r="H4">
-        <v>1.44484548234845</v>
+        <f t="shared" si="1"/>
+        <v>-3.1539999999999999</v>
       </c>
       <c r="I4">
-        <v>0.00202594883764538</v>
+        <f>ROUND(I17,3)</f>
+        <v>-0.95399999999999996</v>
       </c>
       <c r="J4">
-        <v>0.0678363149353465</v>
+        <f>ROUND(J17,3)</f>
+        <v>1.054</v>
       </c>
       <c r="K4">
-        <v>-0.0293387443525021</v>
+        <f>ROUND(K17,3)</f>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="L4">
-        <v>0.953974471534488</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1"/>
+        <f>ROUND(L17,3)</f>
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5">
-        <v>2.32437959929964</v>
+        <f t="shared" si="1"/>
+        <v>1.3089999999999999</v>
       </c>
       <c r="D5">
-        <v>4.11459690207354</v>
-      </c>
-      <c r="K5">
-        <v>0.301003426194962</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>2.4630000000000001</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>-1.054</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>-7.8E-2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>-0.41399999999999998</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="I5">
+        <f>ROUND(I18,3)</f>
+        <v>0.60899999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C6">
-        <v>1.50698819163133</v>
+        <f t="shared" si="1"/>
+        <v>6.9569999999999999</v>
       </c>
       <c r="D6">
-        <v>2.69202707659885</v>
+        <f t="shared" si="1"/>
+        <v>13.496</v>
       </c>
       <c r="E6">
-        <v>0.833845393469247</v>
+        <f t="shared" si="1"/>
+        <v>-0.10299999999999999</v>
       </c>
       <c r="F6">
-        <v>11.9301633846532</v>
+        <f t="shared" si="1"/>
+        <v>2.0840000000000001</v>
       </c>
       <c r="G6">
-        <v>0.800671905794932</v>
+        <f t="shared" si="1"/>
+        <v>2.6080000000000001</v>
       </c>
       <c r="H6">
-        <v>9.91198732038494</v>
+        <f t="shared" si="1"/>
+        <v>2.375</v>
       </c>
       <c r="I6">
-        <v>0.0138469687434326</v>
+        <f>ROUND(I19,3)</f>
+        <v>1.02</v>
       </c>
       <c r="J6">
-        <v>0.569837167391233</v>
+        <f>ROUND(J19,3)</f>
+        <v>-0.61199999999999999</v>
       </c>
       <c r="K6">
-        <v>0.00798692253058476</v>
+        <f>ROUND(K19,3)</f>
+        <v>1E-3</v>
       </c>
       <c r="L6">
-        <v>4.42311810409809</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1"/>
+        <f>ROUND(L19,3)</f>
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C7">
-        <v>0.0383412691349167</v>
+        <f t="shared" si="1"/>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="D7">
-        <v>0.0676909225652484</v>
-      </c>
-      <c r="K7">
-        <v>-0.00322069255132376</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>0.151</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I7">
+        <f>ROUND(I20,3)</f>
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C8">
-        <v>3.76427992973849</v>
+        <f t="shared" si="1"/>
+        <v>3.1280000000000001</v>
       </c>
       <c r="D8">
-        <v>6.67084263113872</v>
+        <f t="shared" si="1"/>
+        <v>5.8339999999999996</v>
       </c>
       <c r="E8">
-        <v>0.379793563543004</v>
+        <f t="shared" si="1"/>
+        <v>-0.214</v>
       </c>
       <c r="F8">
-        <v>3.25753316966075</v>
+        <f t="shared" si="1"/>
+        <v>1.123</v>
       </c>
       <c r="G8">
-        <v>0.425884179356423</v>
+        <f t="shared" si="1"/>
+        <v>1.3759999999999999</v>
       </c>
       <c r="H8">
-        <v>2.9813231565088</v>
+        <f t="shared" si="1"/>
+        <v>0.95799999999999996</v>
       </c>
       <c r="I8">
-        <v>0.00535929629687354</v>
+        <f>ROUND(I21,3)</f>
+        <v>-5.8000000000000003E-2</v>
       </c>
       <c r="J8">
-        <v>0.208657589635569</v>
+        <f>ROUND(J21,3)</f>
+        <v>-0.312</v>
       </c>
       <c r="K8">
-        <v>-0.106188823825785</v>
+        <f>ROUND(K21,3)</f>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>1.74713424122055</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1"/>
+        <f>ROUND(L21,3)</f>
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C9">
-        <v>11.9592247673492</v>
+        <f t="shared" si="1"/>
+        <v>3.149</v>
       </c>
       <c r="D9">
-        <v>20.9864245145032</v>
-      </c>
-      <c r="K9">
-        <v>-0.497954342947623</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>5.6340000000000003</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>-0.78700000000000003</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1.194</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="I9">
+        <f>ROUND(I22,3)</f>
+        <v>-0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C10">
-        <v>0.101517868134867</v>
+        <f t="shared" si="1"/>
+        <v>-0.26500000000000001</v>
       </c>
       <c r="D10">
-        <v>0.0633196535288814</v>
+        <f t="shared" si="1"/>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="E10">
-        <v>-0.0609500979337742</v>
+        <f t="shared" si="1"/>
+        <v>-2.2589999999999999</v>
       </c>
       <c r="F10">
-        <v>4.84329275619321</v>
+        <f t="shared" si="1"/>
+        <v>-0.39</v>
       </c>
       <c r="G10">
-        <v>-0.250374747442361</v>
+        <f t="shared" si="1"/>
+        <v>-0.219</v>
       </c>
       <c r="H10">
-        <v>5.09374738627897</v>
+        <f t="shared" si="1"/>
+        <v>-0.44600000000000001</v>
       </c>
       <c r="I10">
-        <v>-0.00166212804898539</v>
+        <f>ROUND(I23,3)</f>
+        <v>5.6989999999999998</v>
       </c>
       <c r="J10">
-        <v>-0.149924769448857</v>
+        <f>ROUND(J23,3)</f>
+        <v>1.163</v>
       </c>
       <c r="K10">
-        <v>-0.199369150435563</v>
+        <f>ROUND(K23,3)</f>
+        <v>1.2E-2</v>
       </c>
       <c r="L10">
-        <v>2.55975889910371</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1"/>
+        <f>ROUND(L23,3)</f>
+        <v>0.68300000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C11">
-        <v>0.104266862784429</v>
+        <f t="shared" si="1"/>
+        <v>-6.8000000000000005E-2</v>
       </c>
       <c r="D11">
-        <v>0.101699086572095</v>
-      </c>
-      <c r="K11">
-        <v>0.805362214939098</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>-0.35199999999999998</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>-1.5449999999999999</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>-0.16500000000000001</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>-0.51100000000000001</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>-0.38500000000000001</v>
+      </c>
+      <c r="I11">
+        <f>ROUND(I24,3)</f>
+        <v>3.0110000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C12">
-        <v>-0.0288112822857901</v>
+        <f t="shared" si="1"/>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D12">
-        <v>-0.0171232078416467</v>
+        <f t="shared" si="1"/>
+        <v>-0.16900000000000001</v>
       </c>
       <c r="E12">
-        <v>-0.534435546977267</v>
+        <f t="shared" si="1"/>
+        <v>1.4950000000000001</v>
       </c>
       <c r="F12">
-        <v>-4.13710031119576</v>
+        <f t="shared" si="1"/>
+        <v>0.19700000000000001</v>
       </c>
       <c r="G12">
-        <v>-0.603611723385312</v>
+        <f t="shared" si="1"/>
+        <v>0.08</v>
       </c>
       <c r="H12">
-        <v>-4.35502794208627</v>
+        <f t="shared" si="1"/>
+        <v>0.315</v>
       </c>
       <c r="I12">
-        <v>-0.00651550860748081</v>
+        <f>ROUND(I25,3)</f>
+        <v>-3.923</v>
       </c>
       <c r="J12">
-        <v>-0.219088071226124</v>
+        <f>ROUND(J25,3)</f>
+        <v>-0.73199999999999998</v>
       </c>
       <c r="K12">
-        <v>0.0665206985863525</v>
+        <f>ROUND(K25,3)</f>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="L12">
-        <v>-2.98125927856235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="1"/>
+        <f>ROUND(L25,3)</f>
+        <v>-0.36699999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13">
-        <v>-0.00116945048440302</v>
+        <f t="shared" si="1"/>
+        <v>1.2E-2</v>
       </c>
       <c r="D13">
-        <v>-0.000854201081837288</v>
-      </c>
-      <c r="K13">
-        <v>-0.00521950418229762</v>
+        <f t="shared" si="1"/>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I13">
+        <f>ROUND(I26,3)</f>
+        <v>-8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0.237383066549544</v>
+      </c>
+      <c r="D15">
+        <v>8.85757404182895E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.645627394894013</v>
+      </c>
+      <c r="F15">
+        <v>0.22217914788089599</v>
+      </c>
+      <c r="G15">
+        <v>8.7416027255534698E-2</v>
+      </c>
+      <c r="H15">
+        <v>8.16980492899195E-2</v>
+      </c>
+      <c r="I15">
+        <v>-1.57815089566236</v>
+      </c>
+      <c r="J15">
+        <v>-4.0444730641494099E-2</v>
+      </c>
+      <c r="K15">
+        <v>-2.3587016256489999E-4</v>
+      </c>
+      <c r="L15">
+        <v>-1.0380688904255E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0.38193589315856302</v>
+      </c>
+      <c r="D16">
+        <v>0.10304578399057999</v>
+      </c>
+      <c r="E16">
+        <v>-0.123145249837409</v>
+      </c>
+      <c r="F16">
+        <v>0.25855776759355198</v>
+      </c>
+      <c r="G16">
+        <v>-8.2513417223502999E-2</v>
+      </c>
+      <c r="H16">
+        <v>-0.153013236673021</v>
+      </c>
+      <c r="I16">
+        <v>0.11377346662455699</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>-9.4079532282940406</v>
+      </c>
+      <c r="D17">
+        <v>-18.095272435000702</v>
+      </c>
+      <c r="E17">
+        <v>0.11317475615161</v>
+      </c>
+      <c r="F17">
+        <v>-3.0167793202491699</v>
+      </c>
+      <c r="G17">
+        <v>-3.7985753265098201</v>
+      </c>
+      <c r="H17">
+        <v>-3.1536475052323798</v>
+      </c>
+      <c r="I17">
+        <v>-0.95367800259989899</v>
+      </c>
+      <c r="J17">
+        <v>1.0540663530654799</v>
+      </c>
+      <c r="K17">
+        <v>1.14354394257717E-2</v>
+      </c>
+      <c r="L17">
+        <v>0.41026906848028299</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1.3091059974093899</v>
+      </c>
+      <c r="D18">
+        <v>2.4634290568119201</v>
+      </c>
+      <c r="E18">
+        <v>-1.05381141814191</v>
+      </c>
+      <c r="F18">
+        <v>-7.8077730491946204E-2</v>
+      </c>
+      <c r="G18">
+        <v>-0.413599924220238</v>
+      </c>
+      <c r="H18">
+        <v>0.30391163602385002</v>
+      </c>
+      <c r="I18">
+        <v>0.60898483425970795</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>6.95681356870739</v>
+      </c>
+      <c r="D19">
+        <v>13.4961209158381</v>
+      </c>
+      <c r="E19">
+        <v>-0.10325636522416</v>
+      </c>
+      <c r="F19">
+        <v>2.0843181516434801</v>
+      </c>
+      <c r="G19">
+        <v>2.6081123884220299</v>
+      </c>
+      <c r="H19">
+        <v>2.3751852143323702</v>
+      </c>
+      <c r="I19">
+        <v>1.01953618239526</v>
+      </c>
+      <c r="J19">
+        <v>-0.61219797998313297</v>
+      </c>
+      <c r="K19">
+        <v>5.5773896196426997E-4</v>
+      </c>
+      <c r="L19">
+        <v>0.159332680895547</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>8.3504912800042894E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.15081841983081301</v>
+      </c>
+      <c r="E20">
+        <v>3.38059212111858E-3</v>
+      </c>
+      <c r="F20">
+        <v>4.06869156486677E-2</v>
+      </c>
+      <c r="G20">
+        <v>5.3459519798816801E-2</v>
+      </c>
+      <c r="H20">
+        <v>2.4623148944274101E-2</v>
+      </c>
+      <c r="I20">
+        <v>-1.9845976703561301E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3.1283481519807599</v>
+      </c>
+      <c r="D21">
+        <v>5.83425737532749</v>
+      </c>
+      <c r="E21">
+        <v>-0.21352501710580801</v>
+      </c>
+      <c r="F21">
+        <v>1.12320821795062</v>
+      </c>
+      <c r="G21">
+        <v>1.3763894578584499</v>
+      </c>
+      <c r="H21">
+        <v>0.95760486679752899</v>
+      </c>
+      <c r="I21">
+        <v>-5.7512465634568702E-2</v>
+      </c>
+      <c r="J21">
+        <v>-0.31199233672637899</v>
+      </c>
+      <c r="K21">
+        <v>4.7547483587738302E-4</v>
+      </c>
+      <c r="L21">
+        <v>3.90615636907371E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>3.1486157223523699</v>
+      </c>
+      <c r="D22">
+        <v>5.6335954920455498</v>
+      </c>
+      <c r="E22">
+        <v>-0.78677617792199195</v>
+      </c>
+      <c r="F22">
+        <v>1.10168679919898</v>
+      </c>
+      <c r="G22">
+        <v>1.19399691207637</v>
+      </c>
+      <c r="H22">
+        <v>0.80760033117277696</v>
+      </c>
+      <c r="I22">
+        <v>-0.34226963917426001</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>-0.26473354396243098</v>
+      </c>
+      <c r="D23">
+        <v>6.6718315002964296E-2</v>
+      </c>
+      <c r="E23">
+        <v>-2.2591967570757499</v>
+      </c>
+      <c r="F23">
+        <v>-0.38987622788055298</v>
+      </c>
+      <c r="G23">
+        <v>-0.218832219307838</v>
+      </c>
+      <c r="H23">
+        <v>-0.445658257032228</v>
+      </c>
+      <c r="I23">
+        <v>5.6988311736247201</v>
+      </c>
+      <c r="J23">
+        <v>1.16287118684487</v>
+      </c>
+      <c r="K23">
+        <v>1.2387381972706699E-2</v>
+      </c>
+      <c r="L23">
+        <v>0.68269701236751001</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>-6.7729436609979002E-2</v>
+      </c>
+      <c r="D24">
+        <v>-0.35210406418804802</v>
+      </c>
+      <c r="E24">
+        <v>-1.5454137525806599</v>
+      </c>
+      <c r="F24">
+        <v>-0.16501486577740701</v>
+      </c>
+      <c r="G24">
+        <v>-0.51091489780278099</v>
+      </c>
+      <c r="H24">
+        <v>-0.38525668280736097</v>
+      </c>
+      <c r="I24">
+        <v>3.0111994088651302</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>8.1749407675085706E-2</v>
+      </c>
+      <c r="D25">
+        <v>-0.169029725561987</v>
+      </c>
+      <c r="E25">
+        <v>1.4950233241803399</v>
+      </c>
+      <c r="F25">
+        <v>0.19719388649059499</v>
+      </c>
+      <c r="G25">
+        <v>8.0273644640542693E-2</v>
+      </c>
+      <c r="H25">
+        <v>0.314883307469767</v>
+      </c>
+      <c r="I25">
+        <v>-3.9225555633626001</v>
+      </c>
+      <c r="J25">
+        <v>-0.73174893858648904</v>
+      </c>
+      <c r="K25">
+        <v>-1.0712944545350401E-2</v>
+      </c>
+      <c r="L25">
+        <v>-0.36653986174704301</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1.2441101307105001E-2</v>
+      </c>
+      <c r="D26">
+        <v>1.0608284028723E-2</v>
+      </c>
+      <c r="E26">
+        <v>4.0010313339582798E-2</v>
+      </c>
+      <c r="F26">
+        <v>1.18773256692658E-2</v>
+      </c>
+      <c r="G26">
+        <v>1.0373475751463201E-2</v>
+      </c>
+      <c r="H26">
+        <v>6.3818421712132801E-3</v>
+      </c>
+      <c r="I26">
+        <v>-8.5583283903850796E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>